<commit_message>
Mashaba Project with Set Options
</commit_message>
<xml_diff>
--- a/data/ABSA_Cards_Controller.xlsx
+++ b/data/ABSA_Cards_Controller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\vodacom.payment_solution\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD0FDD1-128D-4A9E-B5D3-3F6370A3941C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5695F1CF-4B63-4733-BA78-328E7432EAF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="3000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
     <t>Visa 4038220000353021</t>
   </si>
   <si>
-    <t>NO</t>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -440,7 +440,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C11"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>